<commit_message>
code cleanup and updating data
</commit_message>
<xml_diff>
--- a/data/spleen_data2.xlsx
+++ b/data/spleen_data2.xlsx
@@ -424,8 +424,8 @@
   </sheetPr>
   <dimension ref="A3:AW42"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="X3" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="AK27" activeCellId="0" sqref="AK27"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="O3" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="AI17" activeCellId="0" sqref="AI17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1273,6 +1273,10 @@
       <c r="Y16" s="18"/>
       <c r="Z16" s="18"/>
       <c r="AA16" s="18"/>
+      <c r="AM16" s="0" t="n">
+        <f aca="false">AVERAGE(AM6:AM15)</f>
+        <v>525670.443821212</v>
+      </c>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="4"/>
@@ -1287,7 +1291,10 @@
       <c r="J17" s="4"/>
       <c r="K17" s="4"/>
       <c r="L17" s="4"/>
-      <c r="M17" s="4"/>
+      <c r="M17" s="0" t="n">
+        <f aca="false">AVERAGE(M11:M15)</f>
+        <v>158818.181527273</v>
+      </c>
       <c r="N17" s="4"/>
       <c r="O17" s="5"/>
       <c r="P17" s="5"/>
@@ -1300,13 +1307,20 @@
       <c r="W17" s="4"/>
       <c r="X17" s="4"/>
       <c r="Y17" s="4"/>
-      <c r="Z17" s="4"/>
+      <c r="Z17" s="0" t="n">
+        <f aca="false">AVERAGE(Z11:Z15)</f>
+        <v>166360.028072727</v>
+      </c>
       <c r="AA17" s="4"/>
       <c r="AB17" s="5"/>
       <c r="AC17" s="21"/>
       <c r="AD17" s="5"/>
       <c r="AE17" s="5"/>
       <c r="AF17" s="5"/>
+      <c r="AM17" s="0" t="n">
+        <f aca="false">AVERAGE(AM11:AM15)</f>
+        <v>757312.330909091</v>
+      </c>
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="22"/>

</xml_diff>